<commit_message>
Fix calculation error for ended instances
</commit_message>
<xml_diff>
--- a/Nimble community dashboard.xlsx
+++ b/Nimble community dashboard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instances dashboard" sheetId="1" state="visible" r:id="rId3"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -46,7 +46,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">To leave empty if still running.</t>
+          <t xml:space="preserve">To leave empty if instance is currently running</t>
         </r>
       </text>
     </comment>
@@ -70,7 +70,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">IsActive when there is no instance end date</t>
+          <t xml:space="preserve">IsActive when there is no instance end date.</t>
         </r>
       </text>
     </comment>
@@ -113,9 +113,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t xml:space="preserve">Nimble Instances Dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current cost</t>
   </si>
   <si>
     <t xml:space="preserve">Master address</t>
@@ -145,7 +148,7 @@
     <t xml:space="preserve">isActive</t>
   </si>
   <si>
-    <t xml:space="preserve">Today's instance cost </t>
+    <t xml:space="preserve">Daily instance cost </t>
   </si>
   <si>
     <t xml:space="preserve">Total instance Cost</t>
@@ -211,9 +214,6 @@
     <t xml:space="preserve">My master address:</t>
   </si>
   <si>
-    <t xml:space="preserve">Current cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">qwertzuiopasdfghjklyxcvbnm</t>
   </si>
   <si>
@@ -234,27 +234,28 @@
   <si>
     <t xml:space="preserve">Av. cost / token</t>
   </si>
+  <si>
+    <t xml:space="preserve">Average token cost:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="13">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="General"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yyyy\ hh:mm"/>
-    <numFmt numFmtId="171" formatCode="dd/mm/yy\ hh:mm"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00"/>
-    <numFmt numFmtId="173" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="174" formatCode="#,##0"/>
-    <numFmt numFmtId="175" formatCode="#,##0.000"/>
-    <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="172" formatCode="#,##0"/>
+    <numFmt numFmtId="173" formatCode="#,##0.000"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -278,7 +279,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Roboto Mono"/>
       <family val="0"/>
@@ -301,7 +302,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -332,23 +333,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Roboto Mono"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Roboto Mono"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Roboto Mono"/>
       <family val="0"/>
@@ -360,7 +346,7 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto Mono"/>
       <family val="0"/>
@@ -402,6 +388,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -522,7 +515,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -535,11 +528,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,7 +544,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,7 +568,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,63 +580,71 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -643,19 +652,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -663,23 +664,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,31 +688,39 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="173" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="174" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,10 +730,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -825,7 +830,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9052920" y="123840"/>
+          <a:off x="9042120" y="123840"/>
           <a:ext cx="723600" cy="723600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -867,7 +872,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6959160" y="123840"/>
+          <a:off x="6788880" y="123840"/>
           <a:ext cx="723600" cy="723600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1062,21 +1067,21 @@
   </sheetPr>
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="25.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="25.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="25.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1117,7 +1122,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="6" t="n">
         <f aca="true">NOW()</f>
-        <v>45415.3631973148</v>
+        <v>45416.4638817361</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1130,14 +1135,16 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="7"/>
+      <c r="L3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="8"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1185,41 +1192,41 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="I6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="K6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="L6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="N6" s="11" t="s">
         <v>13</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -1228,43 +1235,43 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="13" t="n">
         <v>45408.5833333333</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="15" t="n">
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="16" t="n">
         <v>4090</v>
       </c>
-      <c r="H7" s="15" t="n">
+      <c r="H7" s="16" t="n">
         <v>0.4</v>
       </c>
-      <c r="I7" s="15" t="n">
+      <c r="I7" s="16" t="n">
         <v>16.7</v>
       </c>
-      <c r="J7" s="16" t="n">
+      <c r="J7" s="17" t="n">
         <f aca="false">H7/(I7*60*60)</f>
         <v>6.65335994677312E-006</v>
       </c>
-      <c r="K7" s="17" t="b">
+      <c r="K7" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D7)),ISBLANK(E7),"")</f>
         <v>1</v>
       </c>
-      <c r="L7" s="18" t="n">
+      <c r="L7" s="19" t="n">
         <f aca="false">IF(K7 = TRUE(), H7*24, "")</f>
         <v>9.6</v>
       </c>
-      <c r="M7" s="19" t="n">
+      <c r="M7" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E7),(NOW()-D7)*H7*24,(F7-D7)*H7*24))</f>
-        <v>65.08910055554</v>
-      </c>
-      <c r="N7" s="15" t="str">
+        <v>75.6532646666513</v>
+      </c>
+      <c r="N7" s="16" t="str">
         <f aca="false">L34</f>
         <v>address1</v>
       </c>
-      <c r="O7" s="20"/>
+      <c r="O7" s="21"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
@@ -1272,43 +1279,43 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="13" t="n">
         <v>45408.6666666667</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="15" t="n">
+      <c r="E8" s="14"/>
+      <c r="F8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="16" t="n">
         <v>3090</v>
       </c>
-      <c r="H8" s="15" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="I8" s="15" t="n">
+      <c r="H8" s="16" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="I8" s="16" t="n">
         <v>10.8</v>
       </c>
-      <c r="J8" s="16" t="n">
+      <c r="J8" s="17" t="n">
         <f aca="false">H8/(I8*60*60)</f>
-        <v>6.43004115226337E-006</v>
-      </c>
-      <c r="K8" s="17" t="b">
+        <v>5.40123456790123E-006</v>
+      </c>
+      <c r="K8" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D8)),ISBLANK(E8),"")</f>
         <v>1</v>
       </c>
-      <c r="L8" s="18" t="n">
+      <c r="L8" s="19" t="n">
         <f aca="false">IF(K8 = TRUE(), H8*24, "")</f>
-        <v>6</v>
-      </c>
-      <c r="M8" s="19" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="M8" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E8),(NOW()-D8)*H8*24,(F8-D8)*H8*24))</f>
-        <v>40.1806879166979</v>
-      </c>
-      <c r="N8" s="15" t="str">
+        <v>39.2979639500164</v>
+      </c>
+      <c r="N8" s="16" t="str">
         <f aca="false">L35</f>
         <v>address2</v>
       </c>
-      <c r="O8" s="20"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
@@ -1316,43 +1323,43 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="21" t="n">
+      <c r="D9" s="13" t="n">
         <v>45411.9583333333</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="15" t="n">
+      <c r="E9" s="14"/>
+      <c r="F9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="16" t="n">
         <v>4090</v>
       </c>
-      <c r="H9" s="15" t="n">
-        <v>0.39</v>
-      </c>
-      <c r="I9" s="15" t="n">
+      <c r="H9" s="16" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="I9" s="16" t="n">
         <v>17.1</v>
       </c>
-      <c r="J9" s="16" t="n">
+      <c r="J9" s="17" t="n">
         <f aca="false">H9/(I9*60*60)</f>
-        <v>6.33528265107213E-006</v>
-      </c>
-      <c r="K9" s="17" t="b">
+        <v>6.82261208576998E-006</v>
+      </c>
+      <c r="K9" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D9)),ISBLANK(E9),"")</f>
         <v>1</v>
       </c>
-      <c r="L9" s="18" t="n">
+      <c r="L9" s="19" t="n">
         <f aca="false">IF(K9 = TRUE(), H9*24, "")</f>
-        <v>9.36</v>
-      </c>
-      <c r="M9" s="19" t="n">
+        <v>10.08</v>
+      </c>
+      <c r="M9" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E9),(NOW()-D9)*H9*24,(F9-D9)*H9*24))</f>
-        <v>31.8718731500034</v>
-      </c>
-      <c r="N9" s="15" t="str">
+        <v>45.4159278999839</v>
+      </c>
+      <c r="N9" s="16" t="str">
         <f aca="false">L36</f>
         <v>address3</v>
       </c>
-      <c r="O9" s="20"/>
+      <c r="O9" s="21"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
@@ -1360,43 +1367,43 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="12" t="n">
+      <c r="D10" s="13" t="n">
         <v>45412.7430555556</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="15" t="n">
+      <c r="E10" s="14"/>
+      <c r="F10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="16" t="n">
         <v>4090</v>
       </c>
-      <c r="H10" s="15" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="I10" s="15" t="n">
+      <c r="H10" s="16" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="I10" s="16" t="n">
         <v>17.5</v>
       </c>
-      <c r="J10" s="16" t="n">
+      <c r="J10" s="17" t="n">
         <f aca="false">H10/(I10*60*60)</f>
-        <v>6.66666666666667E-006</v>
-      </c>
-      <c r="K10" s="17" t="b">
+        <v>6.19047619047619E-006</v>
+      </c>
+      <c r="K10" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D10)),ISBLANK(E10),"")</f>
         <v>1</v>
       </c>
-      <c r="L10" s="18" t="n">
+      <c r="L10" s="19" t="n">
         <f aca="false">IF(K10 = TRUE(), H10*24, "")</f>
-        <v>10.08</v>
-      </c>
-      <c r="M10" s="19" t="n">
+        <v>9.36</v>
+      </c>
+      <c r="M10" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E10),(NOW()-D10)*H10*24,(F10-D10)*H10*24))</f>
-        <v>26.4135557000362</v>
-      </c>
-      <c r="N10" s="15" t="str">
+        <v>34.8269330500153</v>
+      </c>
+      <c r="N10" s="16" t="str">
         <f aca="false">L37</f>
         <v>address4</v>
       </c>
-      <c r="O10" s="20"/>
+      <c r="O10" s="21"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
@@ -1404,43 +1411,43 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="12" t="n">
+      <c r="D11" s="13" t="n">
         <v>45413.5416666667</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="15" t="n">
+      <c r="E11" s="14"/>
+      <c r="F11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="16" t="n">
         <v>3090</v>
       </c>
-      <c r="H11" s="15" t="n">
+      <c r="H11" s="16" t="n">
         <v>0.2</v>
       </c>
-      <c r="I11" s="15" t="n">
+      <c r="I11" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="J11" s="16" t="n">
+      <c r="J11" s="17" t="n">
         <f aca="false">H11/(I11*60*60)</f>
         <v>5.55555555555556E-006</v>
       </c>
-      <c r="K11" s="17" t="b">
+      <c r="K11" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D11)),ISBLANK(E11),"")</f>
         <v>1</v>
       </c>
-      <c r="L11" s="18" t="n">
+      <c r="L11" s="19" t="n">
         <f aca="false">IF(K11 = TRUE(), H11*24, "")</f>
         <v>4.8</v>
       </c>
-      <c r="M11" s="19" t="n">
+      <c r="M11" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E11),(NOW()-D11)*H11*24,(F11-D11)*H11*24))</f>
-        <v>8.74455033335833</v>
-      </c>
-      <c r="N11" s="15" t="str">
+        <v>14.0266323333489</v>
+      </c>
+      <c r="N11" s="16" t="str">
         <f aca="false">L38</f>
         <v>address5</v>
       </c>
-      <c r="O11" s="20"/>
+      <c r="O11" s="21"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
@@ -1448,43 +1455,43 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="21" t="n">
+      <c r="D12" s="13" t="n">
         <v>45414.3958333333</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="15" t="n">
+      <c r="E12" s="14"/>
+      <c r="F12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="16" t="n">
         <v>4090</v>
       </c>
-      <c r="H12" s="15" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="I12" s="15" t="n">
+      <c r="H12" s="16" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I12" s="16" t="n">
         <v>17</v>
       </c>
-      <c r="J12" s="16" t="n">
+      <c r="J12" s="17" t="n">
         <f aca="false">H12/(I12*60*60)</f>
-        <v>7.35294117647059E-006</v>
-      </c>
-      <c r="K12" s="17" t="b">
+        <v>5.88235294117647E-006</v>
+      </c>
+      <c r="K12" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D12)),ISBLANK(E12),"")</f>
         <v>1</v>
       </c>
-      <c r="L12" s="18" t="n">
-        <f aca="false">IF(K12 = TRUE(), H12*24, "")</f>
-        <v>10.8</v>
-      </c>
-      <c r="M12" s="19" t="n">
+      <c r="L12" s="19" t="n">
+        <f aca="false">H12*24</f>
+        <v>8.64</v>
+      </c>
+      <c r="M12" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E12),(NOW()-D12)*H12*24,(F12-D12)*H12*24))</f>
-        <v>10.4502382500039</v>
-      </c>
-      <c r="N12" s="15" t="str">
+        <v>17.8679381999862</v>
+      </c>
+      <c r="N12" s="16" t="str">
         <f aca="false">L39</f>
         <v>address6</v>
       </c>
-      <c r="O12" s="20"/>
+      <c r="O12" s="21"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
@@ -1492,42 +1499,42 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="22" t="n">
+      <c r="D13" s="13" t="n">
         <v>45408.5833333333</v>
       </c>
-      <c r="E13" s="23" t="n">
+      <c r="E13" s="14" t="n">
         <v>45412.6666666667</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="15" t="n">
+      <c r="F13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="16" t="n">
         <v>3090</v>
       </c>
-      <c r="H13" s="15" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="I13" s="15" t="n">
+      <c r="H13" s="16" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="I13" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="J13" s="16" t="n">
+      <c r="J13" s="17" t="n">
         <f aca="false">H13/(I13*60*60)</f>
-        <v>6.94444444444445E-006</v>
-      </c>
-      <c r="K13" s="17" t="b">
+        <v>6.80555555555556E-006</v>
+      </c>
+      <c r="K13" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D13)),ISBLANK(E13),"")</f>
         <v>0</v>
       </c>
-      <c r="L13" s="18" t="str">
-        <f aca="false">IF(K13 = TRUE(), H13*24, "")</f>
-        <v/>
-      </c>
-      <c r="M13" s="19" t="n">
+      <c r="L13" s="19" t="n">
+        <f aca="false">H13*24</f>
+        <v>5.88</v>
+      </c>
+      <c r="M13" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E13),(NOW()-D13)*H13*24,(E13-D13)*H13*24))</f>
-        <v>24.5</v>
-      </c>
-      <c r="N13" s="15"/>
-      <c r="O13" s="20"/>
+        <v>24.01</v>
+      </c>
+      <c r="N13" s="16"/>
+      <c r="O13" s="21"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
@@ -1535,42 +1542,42 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="22" t="n">
+      <c r="D14" s="13" t="n">
         <v>45409.5833333333</v>
       </c>
-      <c r="E14" s="23" t="n">
+      <c r="E14" s="14" t="n">
         <v>45413.0833333333</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="18" t="n">
+      <c r="F14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="19" t="n">
         <v>3090</v>
       </c>
-      <c r="H14" s="18" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="I14" s="18" t="n">
+      <c r="H14" s="19" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="I14" s="19" t="n">
         <v>9.8</v>
       </c>
-      <c r="J14" s="16" t="n">
+      <c r="J14" s="17" t="n">
         <f aca="false">H14/(I14*60*60)</f>
-        <v>5.95238095238095E-006</v>
-      </c>
-      <c r="K14" s="17" t="b">
+        <v>6.23582766439909E-006</v>
+      </c>
+      <c r="K14" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D14)),ISBLANK(E14),"")</f>
         <v>0</v>
       </c>
-      <c r="L14" s="18" t="str">
-        <f aca="false">IF(K14 = TRUE(), H14*24, "")</f>
-        <v/>
-      </c>
-      <c r="M14" s="19" t="n">
+      <c r="L14" s="19" t="n">
+        <f aca="false">H14*24</f>
+        <v>5.28</v>
+      </c>
+      <c r="M14" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E14),(NOW()-D14)*H14*24,(E14-D14)*H14*24))</f>
-        <v>17.64</v>
-      </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="20"/>
+        <v>18.48</v>
+      </c>
+      <c r="N14" s="16"/>
+      <c r="O14" s="21"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
@@ -1578,42 +1585,42 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="22" t="n">
+      <c r="D15" s="13" t="n">
         <v>45411.3888888889</v>
       </c>
-      <c r="E15" s="23" t="n">
+      <c r="E15" s="14" t="n">
         <v>45414.0833333333</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="18" t="n">
+      <c r="F15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="19" t="n">
         <v>4090</v>
       </c>
-      <c r="H15" s="18" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="I15" s="18" t="n">
+      <c r="H15" s="19" t="n">
+        <v>0.399</v>
+      </c>
+      <c r="I15" s="19" t="n">
         <v>17.4</v>
       </c>
-      <c r="J15" s="16" t="n">
+      <c r="J15" s="17" t="n">
         <f aca="false">H15/(I15*60*60)</f>
-        <v>6.38569604086846E-006</v>
-      </c>
-      <c r="K15" s="17" t="b">
+        <v>6.36973180076628E-006</v>
+      </c>
+      <c r="K15" s="18" t="b">
         <f aca="false">IF(NOT(ISBLANK(D15)),ISBLANK(E15),"")</f>
         <v>0</v>
       </c>
-      <c r="L15" s="18" t="str">
-        <f aca="false">IF(K15 = TRUE(), H15*24, "")</f>
-        <v/>
-      </c>
-      <c r="M15" s="19" t="n">
+      <c r="L15" s="19" t="n">
+        <f aca="false">H15*24</f>
+        <v>9.576</v>
+      </c>
+      <c r="M15" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E15),(NOW()-D15)*H15*24,(E15-D15)*H15*24))</f>
-        <v>25.8666666666667</v>
-      </c>
-      <c r="N15" s="15"/>
-      <c r="O15" s="20"/>
+        <v>25.802</v>
+      </c>
+      <c r="N15" s="16"/>
+      <c r="O15" s="21"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
@@ -1621,27 +1628,27 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18" t="str">
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D16)),ISBLANK(E16),"")</f>
         <v/>
       </c>
-      <c r="L16" s="18" t="str">
+      <c r="L16" s="19" t="str">
         <f aca="false">IF(K16 = TRUE(), H16*24, "")</f>
         <v/>
       </c>
-      <c r="M16" s="19" t="n">
+      <c r="M16" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E16),(NOW()-D16)*H16*24,(E16-D16)*H16*24))</f>
         <v>0</v>
       </c>
-      <c r="N16" s="15"/>
-      <c r="O16" s="20"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="21"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
@@ -1649,27 +1656,27 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18" t="str">
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D17)),ISBLANK(E17),"")</f>
         <v/>
       </c>
-      <c r="L17" s="18" t="str">
+      <c r="L17" s="19" t="str">
         <f aca="false">IF(K17 = TRUE(), H17*24, "")</f>
         <v/>
       </c>
-      <c r="M17" s="19" t="n">
+      <c r="M17" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E17),(NOW()-D17)*H17*24,(E17-D17)*H17*24))</f>
         <v>0</v>
       </c>
-      <c r="N17" s="15"/>
-      <c r="O17" s="20"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="21"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
@@ -1677,27 +1684,27 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18" t="str">
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D18)),ISBLANK(E18),"")</f>
         <v/>
       </c>
-      <c r="L18" s="18" t="str">
+      <c r="L18" s="19" t="str">
         <f aca="false">IF(K18 = TRUE(), H18*24, "")</f>
         <v/>
       </c>
-      <c r="M18" s="19" t="n">
+      <c r="M18" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E18),(NOW()-D18)*H18*24,(E18-D18)*H18*24))</f>
         <v>0</v>
       </c>
-      <c r="N18" s="15"/>
-      <c r="O18" s="20"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="21"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
@@ -1705,27 +1712,27 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="str">
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D19)),ISBLANK(E19),"")</f>
         <v/>
       </c>
-      <c r="L19" s="18" t="str">
+      <c r="L19" s="19" t="str">
         <f aca="false">IF(K19 = TRUE(), H19*24, "")</f>
         <v/>
       </c>
-      <c r="M19" s="19" t="n">
+      <c r="M19" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E19),(NOW()-D19)*H19*24,(E19-D19)*H19*24))</f>
         <v>0</v>
       </c>
-      <c r="N19" s="15"/>
-      <c r="O19" s="20"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="21"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
     </row>
@@ -1733,27 +1740,27 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18" t="str">
+      <c r="D20" s="22"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D20)),ISBLANK(E20),"")</f>
         <v/>
       </c>
-      <c r="L20" s="18" t="str">
+      <c r="L20" s="19" t="str">
         <f aca="false">IF(K20 = TRUE(), H20*24, "")</f>
         <v/>
       </c>
-      <c r="M20" s="19" t="n">
+      <c r="M20" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E20),(NOW()-D20)*H20*24,(E20-D20)*H20*24))</f>
         <v>0</v>
       </c>
-      <c r="N20" s="15"/>
-      <c r="O20" s="20"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="21"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
     </row>
@@ -1761,27 +1768,27 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18" t="str">
+      <c r="D21" s="22"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D21)),ISBLANK(E21),"")</f>
         <v/>
       </c>
-      <c r="L21" s="18" t="str">
+      <c r="L21" s="19" t="str">
         <f aca="false">IF(K21 = TRUE(), H21*24, "")</f>
         <v/>
       </c>
-      <c r="M21" s="19" t="n">
+      <c r="M21" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E21),(NOW()-D21)*H21*24,(E21-D21)*H21*24))</f>
         <v>0</v>
       </c>
-      <c r="N21" s="15"/>
-      <c r="O21" s="20"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="21"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
@@ -1789,27 +1796,27 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18" t="str">
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D22)),ISBLANK(E22),"")</f>
         <v/>
       </c>
-      <c r="L22" s="18" t="str">
+      <c r="L22" s="19" t="str">
         <f aca="false">IF(K22 = TRUE(), H22*24, "")</f>
         <v/>
       </c>
-      <c r="M22" s="19" t="n">
+      <c r="M22" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E22),(NOW()-D22)*H22*24,(E22-D22)*H22*24))</f>
         <v>0</v>
       </c>
-      <c r="N22" s="15"/>
-      <c r="O22" s="20"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="21"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
@@ -1817,27 +1824,27 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18" t="str">
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24" t="str">
         <f aca="false">IF(NOT(ISBLANK(D23)),ISBLANK(E23),"")</f>
         <v/>
       </c>
-      <c r="L23" s="18" t="str">
+      <c r="L23" s="19" t="str">
         <f aca="false">IF(K23 = TRUE(), H23*24, "")</f>
         <v/>
       </c>
-      <c r="M23" s="19" t="n">
+      <c r="M23" s="20" t="n">
         <f aca="true">(IF(ISBLANK(E23),(NOW()-D23)*H23*24,(E23-D23)*H23*24))</f>
         <v>0</v>
       </c>
-      <c r="N23" s="15"/>
-      <c r="O23" s="20"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="21"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
@@ -1847,25 +1854,25 @@
       <c r="C24" s="1"/>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26" t="str">
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27" t="str">
         <f aca="false">IF(NOT(ISBLANK(D24)),ISBLANK(E24),"")</f>
         <v/>
       </c>
-      <c r="L24" s="26" t="str">
+      <c r="L24" s="28" t="str">
         <f aca="false">IF(K24 = TRUE(), H24*24, "")</f>
         <v/>
       </c>
-      <c r="M24" s="27" t="n">
+      <c r="M24" s="29" t="n">
         <f aca="true">(IF(ISBLANK(E24),(NOW()-D24)*H24*24,(E24-D24)*H24*24))</f>
         <v>0</v>
       </c>
-      <c r="N24" s="26"/>
-      <c r="O24" s="28"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="30"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
@@ -1988,7 +1995,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1998,7 +2005,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -2029,24 +2036,24 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="29" t="s">
+      <c r="D33" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="29" t="s">
+      <c r="E33" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="31"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="31"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="34"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
@@ -2054,13 +2061,13 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="18" t="n">
-        <f aca="false">E34/24</f>
-        <v>2.11</v>
-      </c>
-      <c r="E34" s="18" t="n">
-        <f aca="false">SUM(L7:L24)</f>
-        <v>50.64</v>
+      <c r="D34" s="24" t="n">
+        <f aca="false">SUMIFS(H7:H24,K7:K24,"="&amp;TRUE())</f>
+        <v>1.98</v>
+      </c>
+      <c r="E34" s="24" t="n">
+        <f aca="false">SUMIFS(L7:L24,K7:K24,"="&amp;TRUE())</f>
+        <v>47.52</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2068,12 +2075,12 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
+      <c r="L34" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
@@ -2081,20 +2088,20 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
+      <c r="L35" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
@@ -2102,20 +2109,20 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
+      <c r="L36" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
@@ -2131,12 +2138,12 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
+      <c r="L37" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
@@ -2152,12 +2159,12 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
+      <c r="L38" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
@@ -2173,12 +2180,12 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
+      <c r="L39" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
@@ -2194,12 +2201,12 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
+      <c r="L40" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
@@ -2215,12 +2222,12 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
+      <c r="L41" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
@@ -2236,12 +2243,12 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
+      <c r="L42" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
@@ -2257,12 +2264,12 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
+      <c r="L43" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
@@ -2278,10 +2285,10 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="34"/>
-      <c r="N44" s="34"/>
-      <c r="O44" s="34"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
+      <c r="O44" s="36"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
@@ -2297,10 +2304,10 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="34"/>
-      <c r="N45" s="34"/>
-      <c r="O45" s="34"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
@@ -2316,10 +2323,10 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="34"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="36"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
@@ -2335,10 +2342,10 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="34"/>
-      <c r="N47" s="34"/>
-      <c r="O47" s="34"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="36"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
@@ -2354,10 +2361,10 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="34"/>
-      <c r="N48" s="34"/>
-      <c r="O48" s="34"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="36"/>
+      <c r="O48" s="36"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
     </row>
@@ -3360,7 +3367,7 @@
     <hyperlink ref="F15" r:id="rId10" display="Vast.ai"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -3378,24 +3385,24 @@
   </sheetPr>
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="0.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="0.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="5.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="5.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3427,14 +3434,14 @@
       <c r="F2" s="1"/>
       <c r="G2" s="5"/>
       <c r="H2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="35"/>
+      <c r="K2" s="37"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="36" t="s">
-        <v>31</v>
+      <c r="M2" s="38" t="s">
+        <v>32</v>
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -3453,9 +3460,9 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="37"/>
+      <c r="M3" s="39"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -3473,11 +3480,11 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
-        <v>32</v>
+      <c r="K4" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="39" t="s">
         <v>33</v>
       </c>
       <c r="N4" s="5"/>
@@ -3499,11 +3506,11 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="38" t="s">
+      <c r="M5" s="40" t="s">
         <v>34</v>
       </c>
       <c r="N5" s="5"/>
-      <c r="O5" s="39"/>
+      <c r="O5" s="41"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -3534,26 +3541,26 @@
       <c r="C7" s="1"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="40" t="s">
-        <v>13</v>
+      <c r="K7" s="42" t="s">
+        <v>14</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="36"/>
+      <c r="M7" s="38"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -3566,93 +3573,95 @@
       <c r="C8" s="1"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="42" t="n">
+      <c r="F8" s="44" t="n">
         <v>45407</v>
       </c>
-      <c r="G8" s="15" t="n">
+      <c r="G8" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="43" t="n">
+      <c r="H8" s="45" t="n">
         <f aca="false">G8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!L7:L18,'Instances dashboard'!D7:D18,"&lt;"&amp;F8,'Instances dashboard'!K7:K18,"="&amp;TRUE())</f>
+      <c r="I8" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F8,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F8,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F8)</f>
         <v>0</v>
       </c>
-      <c r="J8" s="45" t="e">
-        <f aca="false">IF(NOT(ISBLANK(G8)),I8/(H8),"")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="15"/>
+      <c r="J8" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G8)),H8 &lt;&gt; 0),I8/(H8),"")</f>
+        <v/>
+      </c>
+      <c r="K8" s="16"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="37"/>
+      <c r="M8" s="39"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="42" t="n">
+      <c r="F9" s="44" t="n">
         <v>45408</v>
       </c>
-      <c r="G9" s="15" t="n">
+      <c r="G9" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="43" t="n">
+      <c r="H9" s="45" t="n">
         <f aca="false">IF(ISBLANK(G9),"",G9-G8)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!L3:L19,'Instances dashboard'!D3:D19,"&lt;"&amp;F9,'Instances dashboard'!K3:K19,"="&amp;TRUE())</f>
+      <c r="I9" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F9,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F9,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F9)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="45" t="e">
-        <f aca="false">IF(NOT(ISBLANK(G9)),I9/(H9),"")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="15"/>
+      <c r="J9" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G9)),H9 &lt;&gt; 0),I9/(H9),"")</f>
+        <v/>
+      </c>
+      <c r="K9" s="16"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="38"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="39"/>
+      <c r="O9" s="41"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="42" t="n">
+      <c r="F10" s="44" t="n">
         <v>45409</v>
       </c>
-      <c r="G10" s="15" t="n">
-        <v>120</v>
-      </c>
-      <c r="H10" s="43" t="n">
+      <c r="G10" s="16" t="n">
+        <v>100</v>
+      </c>
+      <c r="H10" s="45" t="n">
         <f aca="false">IF(ISBLANK(G10),"",G10-G9)</f>
-        <v>120</v>
-      </c>
-      <c r="I10" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F10,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>15.6</v>
-      </c>
-      <c r="J10" s="45" t="n">
-        <f aca="false">IF(NOT(ISBLANK(G10)),I10/(H10),"")</f>
-        <v>0.13</v>
-      </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="47"/>
+        <v>100</v>
+      </c>
+      <c r="I10" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F10,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F10,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F10)</f>
+        <v>20.52</v>
+      </c>
+      <c r="J10" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G10)),H10 &lt;&gt; 0),I10/(H10),"")</f>
+        <v>0.2052</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="38" t="s">
+        <v>40</v>
+      </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
@@ -3665,28 +3674,28 @@
       <c r="C11" s="1"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="42" t="n">
+      <c r="F11" s="44" t="n">
         <v>45410</v>
       </c>
-      <c r="G11" s="15" t="n">
-        <v>240</v>
-      </c>
-      <c r="H11" s="43" t="n">
+      <c r="G11" s="16" t="n">
+        <v>200</v>
+      </c>
+      <c r="H11" s="45" t="n">
         <f aca="false">IF(ISBLANK(G11),"",G11-G10)</f>
-        <v>120</v>
-      </c>
-      <c r="I11" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F11,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>15.6</v>
-      </c>
-      <c r="J11" s="45" t="n">
-        <f aca="false">IF(NOT(ISBLANK(G11)),I11/(H11),"")</f>
-        <v>0.13</v>
-      </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="I11" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F11,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F11,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F11)</f>
+        <v>25.8</v>
+      </c>
+      <c r="J11" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G11)),H11 &lt;&gt; 0),I11/(H11),"")</f>
+        <v>0.258</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="49"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -3698,27 +3707,30 @@
       <c r="C12" s="1"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="42" t="n">
+      <c r="F12" s="44" t="n">
         <v>45411</v>
       </c>
-      <c r="G12" s="15" t="n">
-        <v>400</v>
-      </c>
-      <c r="H12" s="43" t="n">
+      <c r="G12" s="16" t="n">
+        <v>350</v>
+      </c>
+      <c r="H12" s="45" t="n">
         <f aca="false">IF(ISBLANK(G12),"",G12-G11)</f>
-        <v>160</v>
-      </c>
-      <c r="I12" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F12,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>15.6</v>
-      </c>
-      <c r="J12" s="45" t="n">
-        <f aca="false">IF(NOT(ISBLANK(G12)),I12/(H12),"")</f>
-        <v>0.0975</v>
-      </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="47"/>
+        <v>150</v>
+      </c>
+      <c r="I12" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F12,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F12,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F12)</f>
+        <v>25.8</v>
+      </c>
+      <c r="J12" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G12)),H12 &lt;&gt; 0),I12/(H12),"")</f>
+        <v>0.172</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="50" t="n">
+        <f aca="false">SUM(J8:J44)/COUNT(J8:J44)</f>
+        <v>0.233313469387755</v>
+      </c>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -3731,27 +3743,27 @@
       <c r="C13" s="1"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="42" t="n">
+      <c r="F13" s="44" t="n">
         <v>45412</v>
       </c>
-      <c r="G13" s="15" t="n">
-        <v>550</v>
-      </c>
-      <c r="H13" s="43" t="n">
+      <c r="G13" s="16" t="n">
+        <v>490</v>
+      </c>
+      <c r="H13" s="45" t="n">
         <f aca="false">IF(ISBLANK(G13),"",G13-G12)</f>
-        <v>150</v>
-      </c>
-      <c r="I13" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F13,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>24.96</v>
-      </c>
-      <c r="J13" s="45" t="n">
-        <f aca="false">IF(NOT(ISBLANK(G13)),I13/(H13),"")</f>
-        <v>0.1664</v>
-      </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
+        <v>140</v>
+      </c>
+      <c r="I13" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F13,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F13,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F13)</f>
+        <v>45.456</v>
+      </c>
+      <c r="J13" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G13)),H13 &lt;&gt; 0),I13/(H13),"")</f>
+        <v>0.324685714285714</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="51"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -3764,27 +3776,27 @@
       <c r="C14" s="1"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="42" t="n">
+      <c r="F14" s="44" t="n">
         <v>45413</v>
       </c>
-      <c r="G14" s="15" t="n">
-        <v>750</v>
-      </c>
-      <c r="H14" s="43" t="n">
+      <c r="G14" s="16" t="n">
+        <v>700</v>
+      </c>
+      <c r="H14" s="45" t="n">
         <f aca="false">IF(ISBLANK(G14),"",G14-G13)</f>
-        <v>200</v>
-      </c>
-      <c r="I14" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F14,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>35.04</v>
-      </c>
-      <c r="J14" s="45" t="n">
-        <f aca="false">IF(NOT(ISBLANK(G14)),I14/(H14),"")</f>
-        <v>0.1752</v>
-      </c>
-      <c r="K14" s="48"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="47"/>
+        <v>210</v>
+      </c>
+      <c r="I14" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F14,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F14,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F14)</f>
+        <v>48.936</v>
+      </c>
+      <c r="J14" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G14)),H14 &lt;&gt; 0),I14/(H14),"")</f>
+        <v>0.233028571428571</v>
+      </c>
+      <c r="K14" s="52"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="51"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -3797,27 +3809,27 @@
       <c r="C15" s="1"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="42" t="n">
+      <c r="F15" s="44" t="n">
         <v>45414</v>
       </c>
-      <c r="G15" s="15" t="n">
-        <v>990</v>
-      </c>
-      <c r="H15" s="43" t="n">
+      <c r="G15" s="16" t="n">
+        <v>900</v>
+      </c>
+      <c r="H15" s="45" t="n">
         <f aca="false">IF(ISBLANK(G15),"",G15-G14)</f>
-        <v>240</v>
-      </c>
-      <c r="I15" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F15,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>39.84</v>
-      </c>
-      <c r="J15" s="45" t="n">
-        <f aca="false">IF(NOT(ISBLANK(G15)),I15/(H15),"")</f>
-        <v>0.166</v>
-      </c>
-      <c r="K15" s="15"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
+        <v>200</v>
+      </c>
+      <c r="I15" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F15,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F15,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F15)</f>
+        <v>48.456</v>
+      </c>
+      <c r="J15" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G15)),H15 &lt;&gt; 0),I15/(H15),"")</f>
+        <v>0.24228</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -3830,25 +3842,27 @@
       <c r="C16" s="1"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="42" t="n">
+      <c r="F16" s="44" t="n">
         <v>45415</v>
       </c>
-      <c r="G16" s="15"/>
-      <c r="H16" s="43" t="str">
+      <c r="G16" s="16" t="n">
+        <v>1140</v>
+      </c>
+      <c r="H16" s="45" t="n">
         <f aca="false">IF(ISBLANK(G16),"",G16-G15)</f>
-        <v/>
-      </c>
-      <c r="I16" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F16,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J16" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G16)),I16/(H16),"")</f>
-        <v/>
-      </c>
-      <c r="K16" s="15"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
+        <v>240</v>
+      </c>
+      <c r="I16" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F16,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F16,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F16)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J16" s="47" t="n">
+        <f aca="false">IF(AND(NOT(ISBLANK(G16)),H16 &lt;&gt; 0),I16/(H16),"")</f>
+        <v>0.198</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -3861,25 +3875,25 @@
       <c r="C17" s="1"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="42" t="n">
+      <c r="F17" s="44" t="n">
         <v>45416</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="43" t="str">
+      <c r="G17" s="16"/>
+      <c r="H17" s="45" t="str">
         <f aca="false">IF(ISBLANK(G17),"",G17-G16)</f>
         <v/>
       </c>
-      <c r="I17" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F17,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J17" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G17)),I17/(H17),"")</f>
-        <v/>
-      </c>
-      <c r="K17" s="15"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
+      <c r="I17" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F17,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F17,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F17)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J17" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G17)),H17 &lt;&gt; 0),I17/(H17),"")</f>
+        <v/>
+      </c>
+      <c r="K17" s="16"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -3892,25 +3906,25 @@
       <c r="C18" s="1"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="42" t="n">
+      <c r="F18" s="44" t="n">
         <v>45417</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="43" t="str">
+      <c r="G18" s="16"/>
+      <c r="H18" s="45" t="str">
         <f aca="false">IF(ISBLANK(G18),"",I18/(G18-G17))</f>
         <v/>
       </c>
-      <c r="I18" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F18,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J18" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G18)),I18/(H18),"")</f>
-        <v/>
-      </c>
-      <c r="K18" s="15"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
+      <c r="I18" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F18,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F18,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F18)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J18" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G18)),H18 &lt;&gt; 0),I18/(H18),"")</f>
+        <v/>
+      </c>
+      <c r="K18" s="16"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
@@ -3923,25 +3937,25 @@
       <c r="C19" s="1"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="42" t="n">
+      <c r="F19" s="44" t="n">
         <v>45418</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="43" t="str">
+      <c r="G19" s="16"/>
+      <c r="H19" s="45" t="str">
         <f aca="false">IF(ISBLANK(G19),"",I19/(G19-G18))</f>
         <v/>
       </c>
-      <c r="I19" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F19,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J19" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G19)),I19/(H19),"")</f>
-        <v/>
-      </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
+      <c r="I19" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F19,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F19,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F19)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J19" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G19)),H19 &lt;&gt; 0),I19/(H19),"")</f>
+        <v/>
+      </c>
+      <c r="K19" s="16"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
@@ -3954,25 +3968,25 @@
       <c r="C20" s="1"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="42" t="n">
+      <c r="F20" s="44" t="n">
         <v>45419</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="43" t="str">
+      <c r="G20" s="16"/>
+      <c r="H20" s="45" t="str">
         <f aca="false">IF(ISBLANK(G20),"",I20/(G20-G19))</f>
         <v/>
       </c>
-      <c r="I20" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F20,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J20" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G20)),I20/(H20),"")</f>
-        <v/>
-      </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
+      <c r="I20" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F20,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F20,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F20)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J20" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G20)),H20 &lt;&gt; 0),I20/(H20),"")</f>
+        <v/>
+      </c>
+      <c r="K20" s="16"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -3985,25 +3999,25 @@
       <c r="C21" s="1"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="42" t="n">
+      <c r="F21" s="44" t="n">
         <v>45420</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="43" t="str">
+      <c r="G21" s="16"/>
+      <c r="H21" s="45" t="str">
         <f aca="false">IF(ISBLANK(G21),"",I21/(G21-G20))</f>
         <v/>
       </c>
-      <c r="I21" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F21,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J21" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G21)),I21/(H21),"")</f>
-        <v/>
-      </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
+      <c r="I21" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F21,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F21,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F21)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J21" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G21)),H21 &lt;&gt; 0),I21/(H21),"")</f>
+        <v/>
+      </c>
+      <c r="K21" s="16"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
@@ -4016,25 +4030,25 @@
       <c r="C22" s="1"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="42" t="n">
+      <c r="F22" s="44" t="n">
         <v>45421</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="43" t="str">
+      <c r="G22" s="16"/>
+      <c r="H22" s="45" t="str">
         <f aca="false">IF(ISBLANK(G22),"",I22/(G22-G21))</f>
         <v/>
       </c>
-      <c r="I22" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F22,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J22" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G22)),I22/(H22),"")</f>
-        <v/>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
+      <c r="I22" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F22,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F22,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F22)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J22" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G22)),H22 &lt;&gt; 0),I22/(H22),"")</f>
+        <v/>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -4047,25 +4061,25 @@
       <c r="C23" s="1"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="42" t="n">
+      <c r="F23" s="44" t="n">
         <v>45422</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="43" t="str">
+      <c r="G23" s="16"/>
+      <c r="H23" s="45" t="str">
         <f aca="false">IF(ISBLANK(G23),"",I23/(G23-G22))</f>
         <v/>
       </c>
-      <c r="I23" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F23,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J23" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G23)),I23/(H23),"")</f>
-        <v/>
-      </c>
-      <c r="K23" s="15"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
+      <c r="I23" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F23,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F23,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F23)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J23" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G23)),H23 &lt;&gt; 0),I23/(H23),"")</f>
+        <v/>
+      </c>
+      <c r="K23" s="16"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="P23" s="5"/>
@@ -4078,25 +4092,25 @@
       <c r="C24" s="1"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="42" t="n">
+      <c r="F24" s="44" t="n">
         <v>45423</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="43" t="str">
+      <c r="G24" s="16"/>
+      <c r="H24" s="45" t="str">
         <f aca="false">IF(ISBLANK(G24),"",I24/(G24-G23))</f>
         <v/>
       </c>
-      <c r="I24" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F24,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J24" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G24)),I24/(H24),"")</f>
-        <v/>
-      </c>
-      <c r="K24" s="15"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
+      <c r="I24" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F24,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F24,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F24)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J24" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G24)),H24 &lt;&gt; 0),I24/(H24),"")</f>
+        <v/>
+      </c>
+      <c r="K24" s="16"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
@@ -4109,25 +4123,25 @@
       <c r="C25" s="1"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="42" t="n">
+      <c r="F25" s="44" t="n">
         <v>45424</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="43" t="str">
+      <c r="G25" s="16"/>
+      <c r="H25" s="45" t="str">
         <f aca="false">IF(ISBLANK(G25),"",I25/(G25-G24))</f>
         <v/>
       </c>
-      <c r="I25" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F25,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J25" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G25)),I25/(H25),"")</f>
-        <v/>
-      </c>
-      <c r="K25" s="15"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
+      <c r="I25" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F25,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F25,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F25)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J25" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G25)),H25 &lt;&gt; 0),I25/(H25),"")</f>
+        <v/>
+      </c>
+      <c r="K25" s="16"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
@@ -4140,23 +4154,23 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="42" t="n">
+      <c r="F26" s="44" t="n">
         <v>45425</v>
       </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="43" t="str">
+      <c r="G26" s="16"/>
+      <c r="H26" s="45" t="str">
         <f aca="false">IF(ISBLANK(G26),"",I26/(G26-G25))</f>
         <v/>
       </c>
-      <c r="I26" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F26,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J26" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G26)),I26/(H26),"")</f>
-        <v/>
-      </c>
-      <c r="K26" s="15"/>
+      <c r="I26" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F26,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F26,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F26)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J26" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G26)),H26 &lt;&gt; 0),I26/(H26),"")</f>
+        <v/>
+      </c>
+      <c r="K26" s="16"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
@@ -4171,23 +4185,23 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="42" t="n">
+      <c r="F27" s="44" t="n">
         <v>45426</v>
       </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="43" t="str">
+      <c r="G27" s="16"/>
+      <c r="H27" s="45" t="str">
         <f aca="false">IF(ISBLANK(G27),"",I27/(G27-G26))</f>
         <v/>
       </c>
-      <c r="I27" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F27,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J27" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G27)),I27/(H27),"")</f>
-        <v/>
-      </c>
-      <c r="K27" s="15"/>
+      <c r="I27" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F27,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F27,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F27)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J27" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G27)),H27 &lt;&gt; 0),I27/(H27),"")</f>
+        <v/>
+      </c>
+      <c r="K27" s="16"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -4202,23 +4216,23 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="42" t="n">
+      <c r="F28" s="44" t="n">
         <v>45427</v>
       </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="43" t="str">
+      <c r="G28" s="16"/>
+      <c r="H28" s="45" t="str">
         <f aca="false">IF(ISBLANK(G28),"",I28/(G28-G27))</f>
         <v/>
       </c>
-      <c r="I28" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F28,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J28" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G28)),I28/(H28),"")</f>
-        <v/>
-      </c>
-      <c r="K28" s="15"/>
+      <c r="I28" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F28,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F28,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F28)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J28" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G28)),H28 &lt;&gt; 0),I28/(H28),"")</f>
+        <v/>
+      </c>
+      <c r="K28" s="16"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
@@ -4233,23 +4247,23 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="42" t="n">
+      <c r="F29" s="44" t="n">
         <v>45428</v>
       </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="43" t="str">
+      <c r="G29" s="16"/>
+      <c r="H29" s="45" t="str">
         <f aca="false">IF(ISBLANK(G29),"",I29/(G29-G28))</f>
         <v/>
       </c>
-      <c r="I29" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F29,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J29" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G29)),I29/(H29),"")</f>
-        <v/>
-      </c>
-      <c r="K29" s="15"/>
+      <c r="I29" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F29,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F29,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F29)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J29" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G29)),H29 &lt;&gt; 0),I29/(H29),"")</f>
+        <v/>
+      </c>
+      <c r="K29" s="16"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -4264,23 +4278,23 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="42" t="n">
+      <c r="F30" s="44" t="n">
         <v>45429</v>
       </c>
-      <c r="G30" s="15"/>
-      <c r="H30" s="43" t="str">
+      <c r="G30" s="16"/>
+      <c r="H30" s="45" t="str">
         <f aca="false">IF(ISBLANK(G30),"",I30/(G30-G29))</f>
         <v/>
       </c>
-      <c r="I30" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F30,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J30" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G30)),I30/(H30),"")</f>
-        <v/>
-      </c>
-      <c r="K30" s="15"/>
+      <c r="I30" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F30,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F30,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F30)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J30" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G30)),H30 &lt;&gt; 0),I30/(H30),"")</f>
+        <v/>
+      </c>
+      <c r="K30" s="16"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -4295,23 +4309,23 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="42" t="n">
+      <c r="F31" s="44" t="n">
         <v>45430</v>
       </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="43" t="str">
+      <c r="G31" s="16"/>
+      <c r="H31" s="45" t="str">
         <f aca="false">IF(ISBLANK(G31),"",I31/(G31-G30))</f>
         <v/>
       </c>
-      <c r="I31" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F31,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J31" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G31)),I31/(H31),"")</f>
-        <v/>
-      </c>
-      <c r="K31" s="15"/>
+      <c r="I31" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F31,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F31,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F31)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J31" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G31)),H31 &lt;&gt; 0),I31/(H31),"")</f>
+        <v/>
+      </c>
+      <c r="K31" s="16"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -4326,23 +4340,23 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="42" t="n">
+      <c r="F32" s="44" t="n">
         <v>45431</v>
       </c>
-      <c r="G32" s="15"/>
-      <c r="H32" s="43" t="str">
+      <c r="G32" s="16"/>
+      <c r="H32" s="45" t="str">
         <f aca="false">IF(ISBLANK(G32),"",I32/(G32-G31))</f>
         <v/>
       </c>
-      <c r="I32" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F32,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J32" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G32)),I32/(H32),"")</f>
-        <v/>
-      </c>
-      <c r="K32" s="15"/>
+      <c r="I32" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F32,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F32,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F32)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J32" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G32)),H32 &lt;&gt; 0),I32/(H32),"")</f>
+        <v/>
+      </c>
+      <c r="K32" s="16"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
@@ -4357,23 +4371,23 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="42" t="n">
+      <c r="F33" s="44" t="n">
         <v>45432</v>
       </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="43" t="str">
+      <c r="G33" s="16"/>
+      <c r="H33" s="45" t="str">
         <f aca="false">IF(ISBLANK(G33),"",I33/(G33-G32))</f>
         <v/>
       </c>
-      <c r="I33" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F33,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J33" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G33)),I33/(H33),"")</f>
-        <v/>
-      </c>
-      <c r="K33" s="15"/>
+      <c r="I33" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F33,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F33,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F33)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J33" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G33)),H33 &lt;&gt; 0),I33/(H33),"")</f>
+        <v/>
+      </c>
+      <c r="K33" s="16"/>
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -4388,23 +4402,23 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="42" t="n">
+      <c r="F34" s="44" t="n">
         <v>45433</v>
       </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="43" t="str">
+      <c r="G34" s="16"/>
+      <c r="H34" s="45" t="str">
         <f aca="false">IF(ISBLANK(G34),"",I34/(G34-G33))</f>
         <v/>
       </c>
-      <c r="I34" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F34,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J34" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G34)),I34/(H34),"")</f>
-        <v/>
-      </c>
-      <c r="K34" s="15"/>
+      <c r="I34" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F34,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F34,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F34)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J34" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G34)),H34 &lt;&gt; 0),I34/(H34),"")</f>
+        <v/>
+      </c>
+      <c r="K34" s="16"/>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -4419,23 +4433,23 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="42" t="n">
+      <c r="F35" s="44" t="n">
         <v>45434</v>
       </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="43" t="str">
+      <c r="G35" s="16"/>
+      <c r="H35" s="45" t="str">
         <f aca="false">IF(ISBLANK(G35),"",I35/(G35-G34))</f>
         <v/>
       </c>
-      <c r="I35" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F35,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J35" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G35)),I35/(H35),"")</f>
-        <v/>
-      </c>
-      <c r="K35" s="15"/>
+      <c r="I35" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F35,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F35,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F35)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J35" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G35)),H35 &lt;&gt; 0),I35/(H35),"")</f>
+        <v/>
+      </c>
+      <c r="K35" s="16"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
@@ -4450,23 +4464,23 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
-      <c r="F36" s="42" t="n">
+      <c r="F36" s="44" t="n">
         <v>45435</v>
       </c>
-      <c r="G36" s="15"/>
-      <c r="H36" s="43" t="str">
+      <c r="G36" s="16"/>
+      <c r="H36" s="45" t="str">
         <f aca="false">IF(ISBLANK(G36),"",I36/(G36-G35))</f>
         <v/>
       </c>
-      <c r="I36" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F36,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J36" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G36)),I36/(H36),"")</f>
-        <v/>
-      </c>
-      <c r="K36" s="15"/>
+      <c r="I36" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F36,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F36,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F36)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J36" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G36)),H36 &lt;&gt; 0),I36/(H36),"")</f>
+        <v/>
+      </c>
+      <c r="K36" s="16"/>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
@@ -4481,23 +4495,23 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="42" t="n">
+      <c r="F37" s="44" t="n">
         <v>45436</v>
       </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="43" t="str">
+      <c r="G37" s="16"/>
+      <c r="H37" s="45" t="str">
         <f aca="false">IF(ISBLANK(G37),"",I37/(G37-G36))</f>
         <v/>
       </c>
-      <c r="I37" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F37,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J37" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G37)),I37/(H37),"")</f>
-        <v/>
-      </c>
-      <c r="K37" s="15"/>
+      <c r="I37" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F37,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F37,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F37)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J37" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G37)),H37 &lt;&gt; 0),I37/(H37),"")</f>
+        <v/>
+      </c>
+      <c r="K37" s="16"/>
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
@@ -4512,23 +4526,23 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="42" t="n">
+      <c r="F38" s="44" t="n">
         <v>45437</v>
       </c>
-      <c r="G38" s="15"/>
-      <c r="H38" s="43" t="str">
+      <c r="G38" s="16"/>
+      <c r="H38" s="45" t="str">
         <f aca="false">IF(ISBLANK(G38),"",I38/(G38-G37))</f>
         <v/>
       </c>
-      <c r="I38" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F38,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J38" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G38)),I38/(H38),"")</f>
-        <v/>
-      </c>
-      <c r="K38" s="15"/>
+      <c r="I38" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F38,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F38,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F38)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J38" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G38)),H38 &lt;&gt; 0),I38/(H38),"")</f>
+        <v/>
+      </c>
+      <c r="K38" s="16"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
@@ -4543,23 +4557,23 @@
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="42" t="n">
+      <c r="F39" s="44" t="n">
         <v>45438</v>
       </c>
-      <c r="G39" s="15"/>
-      <c r="H39" s="43" t="str">
+      <c r="G39" s="16"/>
+      <c r="H39" s="45" t="str">
         <f aca="false">IF(ISBLANK(G39),"",I39/(G39-G38))</f>
         <v/>
       </c>
-      <c r="I39" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F39,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J39" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G39)),I39/(H39),"")</f>
-        <v/>
-      </c>
-      <c r="K39" s="15"/>
+      <c r="I39" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F39,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F39,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F39)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J39" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G39)),H39 &lt;&gt; 0),I39/(H39),"")</f>
+        <v/>
+      </c>
+      <c r="K39" s="16"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
@@ -4574,23 +4588,23 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
-      <c r="F40" s="42" t="n">
+      <c r="F40" s="44" t="n">
         <v>45439</v>
       </c>
-      <c r="G40" s="15"/>
-      <c r="H40" s="43" t="str">
+      <c r="G40" s="16"/>
+      <c r="H40" s="45" t="str">
         <f aca="false">IF(ISBLANK(G40),"",I40/(G40-G39))</f>
         <v/>
       </c>
-      <c r="I40" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F40,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J40" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G40)),I40/(H40),"")</f>
-        <v/>
-      </c>
-      <c r="K40" s="15"/>
+      <c r="I40" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F40,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F40,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F40)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J40" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G40)),H40 &lt;&gt; 0),I40/(H40),"")</f>
+        <v/>
+      </c>
+      <c r="K40" s="16"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
@@ -4605,23 +4619,23 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="42" t="n">
+      <c r="F41" s="44" t="n">
         <v>45440</v>
       </c>
-      <c r="G41" s="15"/>
-      <c r="H41" s="43" t="str">
+      <c r="G41" s="16"/>
+      <c r="H41" s="45" t="str">
         <f aca="false">IF(ISBLANK(G41),"",I41/(G41-G40))</f>
         <v/>
       </c>
-      <c r="I41" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F41,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J41" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G41)),I41/(H41),"")</f>
-        <v/>
-      </c>
-      <c r="K41" s="15"/>
+      <c r="I41" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F41,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F41,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F41)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J41" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G41)),H41 &lt;&gt; 0),I41/(H41),"")</f>
+        <v/>
+      </c>
+      <c r="K41" s="16"/>
       <c r="L41" s="5"/>
       <c r="M41" s="5"/>
       <c r="N41" s="5"/>
@@ -4636,23 +4650,23 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="42" t="n">
+      <c r="F42" s="44" t="n">
         <v>45441</v>
       </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="43" t="str">
+      <c r="G42" s="16"/>
+      <c r="H42" s="45" t="str">
         <f aca="false">IF(ISBLANK(G42),"",I42/(G42-G41))</f>
         <v/>
       </c>
-      <c r="I42" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F42,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J42" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G42)),I42/(H42),"")</f>
-        <v/>
-      </c>
-      <c r="K42" s="15"/>
+      <c r="I42" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F42,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F42,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F42)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J42" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G42)),H42 &lt;&gt; 0),I42/(H42),"")</f>
+        <v/>
+      </c>
+      <c r="K42" s="16"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
       <c r="N42" s="5"/>
@@ -4667,23 +4681,23 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="42" t="n">
+      <c r="F43" s="44" t="n">
         <v>45442</v>
       </c>
-      <c r="G43" s="15"/>
-      <c r="H43" s="43" t="str">
+      <c r="G43" s="16"/>
+      <c r="H43" s="45" t="str">
         <f aca="false">IF(ISBLANK(G43),"",I43/(G43-G42))</f>
         <v/>
       </c>
-      <c r="I43" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F43,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J43" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G43)),I43/(H43),"")</f>
-        <v/>
-      </c>
-      <c r="K43" s="15"/>
+      <c r="I43" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F43,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F43,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F43)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J43" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G43)),H43 &lt;&gt; 0),I43/(H43),"")</f>
+        <v/>
+      </c>
+      <c r="K43" s="16"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
@@ -4698,23 +4712,23 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="42" t="n">
+      <c r="F44" s="44" t="n">
         <v>45443</v>
       </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="43" t="str">
+      <c r="G44" s="16"/>
+      <c r="H44" s="45" t="str">
         <f aca="false">IF(ISBLANK(G44),"",I44/(G44-G43))</f>
         <v/>
       </c>
-      <c r="I44" s="44" t="n">
-        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;"&amp;F44,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE())</f>
-        <v>50.64</v>
-      </c>
-      <c r="J44" s="45" t="str">
-        <f aca="false">IF(NOT(ISBLANK(G44)),I44/(H44),"")</f>
-        <v/>
-      </c>
-      <c r="K44" s="15"/>
+      <c r="I44" s="46" t="n">
+        <f aca="false">SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F44,'Instances dashboard'!$K$7:$K$18,"="&amp;TRUE()) + SUMIFS('Instances dashboard'!$L$7:$L$18,'Instances dashboard'!$K$7:$K$18,"="&amp;FALSE(),'Instances dashboard'!$D$7:$D$18,"&lt;="&amp;F44,'Instances dashboard'!$E$7:$E$18,"&gt;="&amp;F44)</f>
+        <v>47.52</v>
+      </c>
+      <c r="J44" s="47" t="str">
+        <f aca="false">IF(AND(NOT(ISBLANK(G44)),H44 &lt;&gt; 0),I44/(H44),"")</f>
+        <v/>
+      </c>
+      <c r="K44" s="16"/>
       <c r="L44" s="5"/>
       <c r="M44" s="5"/>
       <c r="N44" s="5"/>
@@ -5848,7 +5862,7 @@
     <hyperlink ref="M5" r:id="rId2" display="Check balance"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>